<commit_message>
added NOP, LDA, OUT and HLT to instruction set
</commit_message>
<xml_diff>
--- a/Instruction-Set-Generator/Instruction_Set_Microcode.xlsx
+++ b/Instruction-Set-Generator/Instruction_Set_Microcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Ben-Eater-8-Bit-Computer\Instruction-Set-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092E371A-1C12-4054-8CA3-67FA78B25C29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE6CD39-C99A-4EB3-AAF1-4F47C36DFFD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DC0BBB7-A731-4CCE-804E-F7FA7138307F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Instruction Name</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Instruction Number</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>OUT</t>
   </si>
 </sst>
 </file>
@@ -222,12 +231,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,6 +239,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -603,8 +612,8 @@
   <dimension ref="A1:Y82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z10" sqref="Z10"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,44 +645,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="18" t="s">
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="18" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="20"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="18"/>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="22"/>
       <c r="C2" s="5" t="s">
         <v>2</v>
@@ -734,6 +743,9 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B3" s="4">
         <v>0</v>
       </c>
@@ -1094,6 +1106,9 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
@@ -1297,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="8">
         <v>0</v>
@@ -1306,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="8">
         <v>0</v>
@@ -1374,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="8">
         <v>0</v>
@@ -1383,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="8">
         <v>0</v>
@@ -6164,6 +6179,9 @@
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B73" s="4">
         <v>14</v>
       </c>
@@ -6385,7 +6403,7 @@
         <v>0</v>
       </c>
       <c r="R75" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S75" s="8">
         <v>0</v>
@@ -6397,7 +6415,7 @@
         <v>0</v>
       </c>
       <c r="V75" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W75" s="8">
         <v>0</v>
@@ -6554,6 +6572,9 @@
       </c>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B78" s="4">
         <v>15</v>
       </c>
@@ -6754,7 +6775,7 @@
         <v>0</v>
       </c>
       <c r="K80" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L80" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
added STA, LDI, JMP instructions
</commit_message>
<xml_diff>
--- a/Instruction-Set-Generator/Instruction_Set_Microcode.xlsx
+++ b/Instruction-Set-Generator/Instruction_Set_Microcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Ben-Eater-8-Bit-Computer\Instruction-Set-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5429DF86-3875-4E45-828F-E9FE4B429389}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF87D79E-06BE-410F-B9E2-97225278121D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6DC0BBB7-A731-4CCE-804E-F7FA7138307F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Instruction Name</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>SUB</t>
+  </si>
+  <si>
+    <t>STA</t>
+  </si>
+  <si>
+    <t>LDI</t>
+  </si>
+  <si>
+    <t>JMP</t>
   </si>
 </sst>
 </file>
@@ -618,8 +627,8 @@
   <dimension ref="A1:Y82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T23" sqref="T23"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,6 +2300,9 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B23" s="4">
         <v>4</v>
       </c>
@@ -2494,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="8">
         <v>0</v>
@@ -2503,7 +2515,7 @@
         <v>0</v>
       </c>
       <c r="O25" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" s="8">
         <v>0</v>
@@ -2568,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="8">
         <v>0</v>
@@ -2583,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="8">
         <v>0</v>
@@ -2681,6 +2693,9 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B28" s="4">
         <v>5</v>
       </c>
@@ -2893,13 +2908,13 @@
         <v>0</v>
       </c>
       <c r="O30" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="8">
         <v>0</v>
       </c>
       <c r="Q30" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30" s="8">
         <v>0</v>
@@ -3071,6 +3086,9 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B33" s="4">
         <v>6</v>
       </c>
@@ -3283,7 +3301,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="8">
         <v>0</v>
@@ -3313,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="Y35" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>